<commit_message>
Đẩy code lại để cả team cung fix
</commit_message>
<xml_diff>
--- a/DanhSach.xlsx
+++ b/DanhSach.xlsx
@@ -12,330 +12,348 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="114">
   <si>
     <t>Danh Sách Sản Phẩm</t>
   </si>
   <si>
-    <t>SPCT02</t>
-  </si>
-  <si>
-    <t>5901234123457</t>
-  </si>
-  <si>
-    <t>Thấm hút mồ hôi, độ co giãn tốt</t>
-  </si>
-  <si>
-    <t>Áo phông cổ tròn</t>
+    <t>SPCT45</t>
+  </si>
+  <si>
+    <t>8934674012415</t>
+  </si>
+  <si>
+    <t>Thoáng khí, chất liệu cao cấp</t>
+  </si>
+  <si>
+    <t>Áo Nỉ Crewneck</t>
+  </si>
+  <si>
+    <t>Fila</t>
+  </si>
+  <si>
+    <t>LOKITA</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Vàng</t>
+  </si>
+  <si>
+    <t>Vải Gore-Tex</t>
+  </si>
+  <si>
+    <t>SPCT67</t>
+  </si>
+  <si>
+    <t>9780486996844</t>
+  </si>
+  <si>
+    <t>Chống mài mòn, thoáng khí</t>
+  </si>
+  <si>
+    <t>Áo Sweeter cổ lọ</t>
+  </si>
+  <si>
+    <t>Kappa</t>
+  </si>
+  <si>
+    <t>THEFACE</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Trắng</t>
+  </si>
+  <si>
+    <t>SPCT68</t>
+  </si>
+  <si>
+    <t>1234567890128</t>
+  </si>
+  <si>
+    <t>Không nhăn, không xù, không phai</t>
+  </si>
+  <si>
+    <t>Áo gile cổ chữ V</t>
+  </si>
+  <si>
+    <t>Puma</t>
+  </si>
+  <si>
+    <t>ECHOPE</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Tím</t>
+  </si>
+  <si>
+    <t>Vải Cotton</t>
+  </si>
+  <si>
+    <t>SPCT10</t>
+  </si>
+  <si>
+    <t>Áo phao gió</t>
+  </si>
+  <si>
+    <t>Vải Nylon</t>
+  </si>
+  <si>
+    <t>SPCT49</t>
+  </si>
+  <si>
+    <t>SPCT57</t>
+  </si>
+  <si>
+    <t>SPCT51</t>
+  </si>
+  <si>
+    <t>SPCT07</t>
+  </si>
+  <si>
+    <t>1321412341239</t>
+  </si>
+  <si>
+    <t>Chất liệu cao cấp</t>
+  </si>
+  <si>
+    <t>Áo sơ mi Linen</t>
   </si>
   <si>
     <t>Nike</t>
   </si>
   <si>
+    <t>Xanh dương</t>
+  </si>
+  <si>
+    <t>Vải Polyester</t>
+  </si>
+  <si>
+    <t>SPCT08</t>
+  </si>
+  <si>
+    <t>SPCT09</t>
+  </si>
+  <si>
+    <t>SPCT11</t>
+  </si>
+  <si>
+    <t>SPCT12</t>
+  </si>
+  <si>
+    <t>SPCT13</t>
+  </si>
+  <si>
+    <t>SPCT14</t>
+  </si>
+  <si>
+    <t>SPCT15</t>
+  </si>
+  <si>
+    <t>SPCT16</t>
+  </si>
+  <si>
+    <t>SPCT17</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Thoáng khí, không phai màu</t>
+  </si>
+  <si>
+    <t>Áo Hoodie zip</t>
+  </si>
+  <si>
+    <t>SPCT18</t>
+  </si>
+  <si>
+    <t>SPCT19</t>
+  </si>
+  <si>
+    <t>SPCT22</t>
+  </si>
+  <si>
+    <t>Rộng rãi, thoải mái</t>
+  </si>
+  <si>
+    <t>SPCT23</t>
+  </si>
+  <si>
+    <t>2131241241255</t>
+  </si>
+  <si>
+    <t>Thoáng khí, thấm hút mồ hôi</t>
+  </si>
+  <si>
+    <t>Áo Vest công sở</t>
+  </si>
+  <si>
     <t>HANDMADE</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>Xanh</t>
-  </si>
-  <si>
-    <t>Vải Nylon</t>
-  </si>
-  <si>
-    <t>SPCT03</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>SPCT04</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>SPCT05</t>
-  </si>
-  <si>
-    <t>BASIC</t>
-  </si>
-  <si>
-    <t>XL</t>
+    <t>SPCT24</t>
+  </si>
+  <si>
+    <t>SPCT25</t>
+  </si>
+  <si>
+    <t>SPCT26</t>
+  </si>
+  <si>
+    <t>SPCT27</t>
+  </si>
+  <si>
+    <t>Độ co giãn tốt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Áo Khoác Bomber </t>
+  </si>
+  <si>
+    <t>SPCT28</t>
+  </si>
+  <si>
+    <t>Đen</t>
+  </si>
+  <si>
+    <t>Vải Spandex</t>
+  </si>
+  <si>
+    <t>SPCT29</t>
+  </si>
+  <si>
+    <t>Li ning</t>
+  </si>
+  <si>
+    <t>Đỏ</t>
+  </si>
+  <si>
+    <t>SPCT30</t>
+  </si>
+  <si>
+    <t>Chất liệu cao cấp, bền bỉ</t>
+  </si>
+  <si>
+    <t>Áo Jean dài</t>
+  </si>
+  <si>
+    <t>Uniqlo</t>
+  </si>
+  <si>
+    <t>PEONY</t>
+  </si>
+  <si>
+    <t>Nâu</t>
+  </si>
+  <si>
+    <t>Vải Bamboo</t>
+  </si>
+  <si>
+    <t>SPCT31</t>
+  </si>
+  <si>
+    <t>SPCT32</t>
+  </si>
+  <si>
+    <t>SPCT43</t>
+  </si>
+  <si>
+    <t>Ấp áp, dày dặn</t>
+  </si>
+  <si>
+    <t>Áo Polo Rugby</t>
+  </si>
+  <si>
+    <t>Adidas</t>
+  </si>
+  <si>
+    <t>SPCT44</t>
+  </si>
+  <si>
+    <t>SPCT46</t>
+  </si>
+  <si>
+    <t>SPCT47</t>
+  </si>
+  <si>
+    <t>SPCT48</t>
+  </si>
+  <si>
+    <t>SPCT50</t>
+  </si>
+  <si>
+    <t>SPCT52</t>
+  </si>
+  <si>
+    <t>SPCT53</t>
+  </si>
+  <si>
+    <t>SPCT54</t>
+  </si>
+  <si>
+    <t>SPCT55</t>
   </si>
   <si>
     <t>SPCT56</t>
   </si>
   <si>
-    <t>1234567890128</t>
-  </si>
-  <si>
-    <t>Không nhăn, không xù, không phai</t>
-  </si>
-  <si>
-    <t>Áo phao gió</t>
-  </si>
-  <si>
-    <t>Puma</t>
-  </si>
-  <si>
-    <t>ECHOPE</t>
-  </si>
-  <si>
-    <t>Tím</t>
-  </si>
-  <si>
-    <t>Vải Cotton</t>
-  </si>
-  <si>
-    <t>SPCT57</t>
-  </si>
-  <si>
-    <t>SPCT034</t>
-  </si>
-  <si>
-    <t>1321412341239</t>
-  </si>
-  <si>
-    <t>Chất liệu cao cấp</t>
-  </si>
-  <si>
-    <t>Áo sơ mi Linen</t>
-  </si>
-  <si>
-    <t>Adidas</t>
-  </si>
-  <si>
-    <t>Đỏ</t>
-  </si>
-  <si>
-    <t>SPCT07</t>
-  </si>
-  <si>
-    <t>Xanh dương</t>
-  </si>
-  <si>
-    <t>Vải Polyester</t>
-  </si>
-  <si>
-    <t>SPCT08</t>
-  </si>
-  <si>
-    <t>SPCT09</t>
-  </si>
-  <si>
-    <t>SPCT10</t>
-  </si>
-  <si>
-    <t>SPCT11</t>
-  </si>
-  <si>
-    <t>8934674012415</t>
-  </si>
-  <si>
-    <t>Thoáng khí, chất liệu cao cấp</t>
-  </si>
-  <si>
-    <t>Áo Nỉ Crewneck</t>
-  </si>
-  <si>
-    <t>Fila</t>
-  </si>
-  <si>
-    <t>LOKITA</t>
-  </si>
-  <si>
-    <t>Vàng</t>
-  </si>
-  <si>
-    <t>Vải Gore-Tex</t>
-  </si>
-  <si>
-    <t>SPCT12</t>
-  </si>
-  <si>
-    <t>SPCT13</t>
-  </si>
-  <si>
-    <t>SPCT14</t>
-  </si>
-  <si>
-    <t>9780486996844</t>
-  </si>
-  <si>
-    <t>Chống mài mòn, thoáng khí</t>
-  </si>
-  <si>
-    <t>Áo gile cổ chữ V</t>
-  </si>
-  <si>
-    <t>Kappa</t>
-  </si>
-  <si>
-    <t>THEFACE</t>
-  </si>
-  <si>
-    <t>Trắng</t>
-  </si>
-  <si>
-    <t>SPCT15</t>
-  </si>
-  <si>
-    <t>SPCT16</t>
-  </si>
-  <si>
-    <t>SPCT17</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Thoáng khí, không phai màu</t>
-  </si>
-  <si>
-    <t>Áo Hoodie zip</t>
-  </si>
-  <si>
-    <t>SPCT18</t>
-  </si>
-  <si>
-    <t>SPCT19</t>
-  </si>
-  <si>
-    <t>SPCT20</t>
-  </si>
-  <si>
-    <t>Rộng rãi, thoải mái</t>
-  </si>
-  <si>
-    <t>Áo Sweeter cổ lọ</t>
-  </si>
-  <si>
-    <t>SPCT21</t>
-  </si>
-  <si>
-    <t>SPCT22</t>
-  </si>
-  <si>
-    <t>SPCT23</t>
-  </si>
-  <si>
-    <t>Thoáng khí, thấm hút mồ hôi</t>
-  </si>
-  <si>
-    <t>Áo Vest công sở</t>
-  </si>
-  <si>
-    <t>SPCT24</t>
-  </si>
-  <si>
-    <t>SPCT25</t>
-  </si>
-  <si>
-    <t>SPCT26</t>
-  </si>
-  <si>
-    <t>SPCT27</t>
-  </si>
-  <si>
-    <t>Độ co giãn tốt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Áo Khoác Bomber </t>
-  </si>
-  <si>
-    <t>SPCT28</t>
-  </si>
-  <si>
-    <t>Đen</t>
-  </si>
-  <si>
-    <t>Vải Spandex</t>
-  </si>
-  <si>
-    <t>SPCT29</t>
-  </si>
-  <si>
-    <t>Li ning</t>
-  </si>
-  <si>
-    <t>SPCT30</t>
-  </si>
-  <si>
-    <t>Chất liệu cao cấp, bền bỉ</t>
-  </si>
-  <si>
-    <t>Áo Jean dài</t>
-  </si>
-  <si>
-    <t>Uniqlo</t>
-  </si>
-  <si>
-    <t>PEONY</t>
-  </si>
-  <si>
-    <t>Nâu</t>
-  </si>
-  <si>
-    <t>Vải Bamboo</t>
-  </si>
-  <si>
-    <t>SPCT31</t>
-  </si>
-  <si>
-    <t>SPCT32</t>
-  </si>
-  <si>
-    <t>SPCT43</t>
-  </si>
-  <si>
-    <t>Ấp áp, dày dặn</t>
-  </si>
-  <si>
-    <t>Áo Polo Rugby</t>
-  </si>
-  <si>
-    <t>SPCT44</t>
-  </si>
-  <si>
-    <t>SPCT45</t>
-  </si>
-  <si>
-    <t>SPCT46</t>
-  </si>
-  <si>
-    <t>SPCT47</t>
-  </si>
-  <si>
-    <t>123457656456</t>
-  </si>
-  <si>
-    <t>SPCT48</t>
-  </si>
-  <si>
-    <t>SPCT49</t>
-  </si>
-  <si>
-    <t>SPCT50</t>
-  </si>
-  <si>
-    <t>13214123412</t>
-  </si>
-  <si>
-    <t>SPCT51</t>
-  </si>
-  <si>
-    <t>SPCT52</t>
-  </si>
-  <si>
-    <t>SPCT53</t>
-  </si>
-  <si>
-    <t>SPCT54</t>
-  </si>
-  <si>
-    <t>SPCT55</t>
+    <t>SPCT58</t>
+  </si>
+  <si>
+    <t>SPCT59</t>
+  </si>
+  <si>
+    <t>SPCT60</t>
+  </si>
+  <si>
+    <t>SPCT61</t>
+  </si>
+  <si>
+    <t>SPCT62</t>
+  </si>
+  <si>
+    <t>SPCT63</t>
+  </si>
+  <si>
+    <t>SPCT64</t>
+  </si>
+  <si>
+    <t>SPCT65</t>
+  </si>
+  <si>
+    <t>SPCT66</t>
+  </si>
+  <si>
+    <t>SPCT69</t>
+  </si>
+  <si>
+    <t>Chống mài mòn, thoáng khí1</t>
+  </si>
+  <si>
+    <t>Wika</t>
+  </si>
+  <si>
+    <t>UNIQLO</t>
+  </si>
+  <si>
+    <t>SPCT70</t>
+  </si>
+  <si>
+    <t>SPCT71</t>
+  </si>
+  <si>
+    <t>SPCT72</t>
+  </si>
+  <si>
+    <t>SPCT73</t>
+  </si>
+  <si>
+    <t>SPCT74</t>
   </si>
 </sst>
 </file>
@@ -380,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:N66"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -405,7 +423,7 @@
         <v>3</v>
       </c>
       <c r="E2" t="n">
-        <v>17.0</v>
+        <v>12.0</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
@@ -426,10 +444,10 @@
         <v>9</v>
       </c>
       <c r="L2" t="n">
-        <v>70000.0</v>
+        <v>40000.0</v>
       </c>
       <c r="M2" t="n">
-        <v>105000.0</v>
+        <v>60000.0</v>
       </c>
       <c r="N2" t="b">
         <v>1</v>
@@ -443,37 +461,37 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E3" t="n">
-        <v>19.0</v>
+        <v>1.0</v>
       </c>
       <c r="F3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="K3" t="s">
         <v>9</v>
       </c>
       <c r="L3" t="n">
-        <v>6000.0</v>
+        <v>120000.0</v>
       </c>
       <c r="M3" t="n">
-        <v>90000.0</v>
+        <v>180000.0</v>
       </c>
       <c r="N3" t="b">
         <v>1</v>
@@ -484,43 +502,43 @@
         <v>13.0</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="H4" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="I4" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="J4" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="K4" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="L4" t="n">
-        <v>60000.0</v>
+        <v>100000.0</v>
       </c>
       <c r="M4" t="n">
-        <v>90000.0</v>
+        <v>150000.0</v>
       </c>
       <c r="N4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -528,40 +546,40 @@
         <v>14.0</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="E5" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="F5" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J5" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="K5" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="L5" t="n">
-        <v>80000.0</v>
+        <v>90000.0</v>
       </c>
       <c r="M5" t="n">
-        <v>120000.0</v>
+        <v>135000.0</v>
       </c>
       <c r="N5" t="b">
         <v>1</v>
@@ -572,43 +590,43 @@
         <v>15.0</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>141.0</v>
+        <v>0.0</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="J6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="K6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L6" t="n">
-        <v>100000.0</v>
+        <v>120000.0</v>
       </c>
       <c r="M6" t="n">
-        <v>150000.0</v>
+        <v>180000.0</v>
       </c>
       <c r="N6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -616,40 +634,40 @@
         <v>16.0</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E7" t="n">
-        <v>14.0</v>
+        <v>204.0</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I7" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="J7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="K7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L7" t="n">
-        <v>100000.0</v>
+        <v>120000.0</v>
       </c>
       <c r="M7" t="n">
-        <v>2.2222222E7</v>
+        <v>180000.0</v>
       </c>
       <c r="N7" t="b">
         <v>1</v>
@@ -660,34 +678,34 @@
         <v>17.0</v>
       </c>
       <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" t="s">
         <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" t="n">
-        <v>222.0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" t="s">
-        <v>31</v>
-      </c>
-      <c r="K8" t="s">
-        <v>24</v>
       </c>
       <c r="L8" t="n">
         <v>120000.0</v>
@@ -704,34 +722,34 @@
         <v>18.0</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="E9" t="n">
-        <v>8.0</v>
+        <v>11.0</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="G9" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="H9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I9" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J9" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="K9" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L9" t="n">
         <v>120000.0</v>
@@ -748,34 +766,34 @@
         <v>19.0</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E10" t="n">
         <v>14.0</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="G10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I10" t="s">
         <v>7</v>
       </c>
       <c r="J10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L10" t="n">
         <v>100000.0</v>
@@ -792,34 +810,34 @@
         <v>20.0</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E11" t="n">
-        <v>27.0</v>
+        <v>1.0</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I11" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L11" t="n">
         <v>100000.0</v>
@@ -836,34 +854,34 @@
         <v>21.0</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E12" t="n">
-        <v>1.0</v>
+        <v>23.0</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="G12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I12" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="J12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K12" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="L12" t="n">
         <v>90000.0</v>
@@ -880,34 +898,34 @@
         <v>22.0</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="E13" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="F13" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="G13" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="H13" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="I13" t="s">
         <v>7</v>
       </c>
       <c r="J13" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="K13" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="L13" t="n">
         <v>40000.0</v>
@@ -924,34 +942,34 @@
         <v>23.0</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="E14" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="F14" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="G14" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="H14" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="I14" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J14" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="K14" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="L14" t="n">
         <v>40000.0</v>
@@ -968,34 +986,34 @@
         <v>24.0</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="E15" t="n">
         <v>7.0</v>
       </c>
       <c r="F15" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="G15" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="H15" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="I15" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="J15" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="K15" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="L15" t="n">
         <v>60000.0</v>
@@ -1012,34 +1030,34 @@
         <v>25.0</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="E16" t="n">
-        <v>18.0</v>
+        <v>20.0</v>
       </c>
       <c r="F16" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="G16" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="H16" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="I16" t="s">
         <v>7</v>
       </c>
       <c r="J16" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="K16" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L16" t="n">
         <v>100000.0</v>
@@ -1056,34 +1074,34 @@
         <v>26.0</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="E17" t="n">
-        <v>17.0</v>
+        <v>2.0</v>
       </c>
       <c r="F17" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="G17" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="H17" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="I17" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J17" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="K17" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L17" t="n">
         <v>100000.0</v>
@@ -1100,34 +1118,34 @@
         <v>27.0</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="E18" t="n">
-        <v>8.0</v>
+        <v>12.0</v>
       </c>
       <c r="F18" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="G18" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="H18" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="I18" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="J18" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="K18" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L18" t="n">
         <v>120000.0</v>
@@ -1144,34 +1162,34 @@
         <v>28.0</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E19" t="n">
         <v>10.0</v>
       </c>
       <c r="F19" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="G19" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="H19" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="I19" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J19" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="K19" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L19" t="n">
         <v>80000.0</v>
@@ -1188,34 +1206,34 @@
         <v>29.0</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E20" t="n">
         <v>13.0</v>
       </c>
       <c r="F20" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="G20" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="H20" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="I20" t="s">
         <v>7</v>
       </c>
       <c r="J20" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="K20" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L20" t="n">
         <v>60000.0</v>
@@ -1232,34 +1250,34 @@
         <v>30.0</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E21" t="n">
         <v>13.0</v>
       </c>
       <c r="F21" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="G21" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="H21" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="I21" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J21" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="K21" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L21" t="n">
         <v>80000.0</v>
@@ -1276,40 +1294,40 @@
         <v>31.0</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="E22" t="n">
-        <v>20.0</v>
+        <v>101.0</v>
       </c>
       <c r="F22" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="G22" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="H22" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="I22" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J22" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="K22" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="L22" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="M22" t="n">
         <v>60000.0</v>
-      </c>
-      <c r="M22" t="n">
-        <v>90000.0</v>
       </c>
       <c r="N22" t="b">
         <v>1</v>
@@ -1320,40 +1338,40 @@
         <v>32.0</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="E23" t="n">
-        <v>18.0</v>
+        <v>11.0</v>
       </c>
       <c r="F23" t="s">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="G23" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="H23" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="I23" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="J23" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="K23" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="L23" t="n">
+        <v>40000.0</v>
+      </c>
+      <c r="M23" t="n">
         <v>60000.0</v>
-      </c>
-      <c r="M23" t="n">
-        <v>90000.0</v>
       </c>
       <c r="N23" t="b">
         <v>1</v>
@@ -1364,34 +1382,34 @@
         <v>33.0</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D24" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E24" t="n">
         <v>12.0</v>
       </c>
       <c r="F24" t="s">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="G24" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="H24" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="I24" t="s">
         <v>7</v>
       </c>
       <c r="J24" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="K24" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L24" t="n">
         <v>80000.0</v>
@@ -1408,34 +1426,34 @@
         <v>34.0</v>
       </c>
       <c r="B25" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="C25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" t="s">
         <v>58</v>
       </c>
-      <c r="D25" t="s">
-        <v>69</v>
-      </c>
       <c r="E25" t="n">
-        <v>10.0</v>
+        <v>101.0</v>
       </c>
       <c r="F25" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="G25" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="H25" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="I25" t="s">
         <v>7</v>
       </c>
       <c r="J25" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="K25" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="L25" t="n">
         <v>80000.0</v>
@@ -1452,34 +1470,34 @@
         <v>35.0</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" t="s">
         <v>58</v>
-      </c>
-      <c r="D26" t="s">
-        <v>69</v>
       </c>
       <c r="E26" t="n">
         <v>10.0</v>
       </c>
       <c r="F26" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="G26" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H26" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="I26" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J26" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="K26" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L26" t="n">
         <v>80000.0</v>
@@ -1496,34 +1514,34 @@
         <v>36.0</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" t="s">
         <v>58</v>
-      </c>
-      <c r="D27" t="s">
-        <v>69</v>
       </c>
       <c r="E27" t="n">
         <v>8.0</v>
       </c>
       <c r="F27" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="G27" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H27" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="I27" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="J27" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="K27" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L27" t="n">
         <v>80000.0</v>
@@ -1540,34 +1558,34 @@
         <v>37.0</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" t="s">
         <v>58</v>
-      </c>
-      <c r="D28" t="s">
-        <v>69</v>
       </c>
       <c r="E28" t="n">
         <v>8.0</v>
       </c>
       <c r="F28" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="G28" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H28" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="I28" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J28" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="K28" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L28" t="n">
         <v>100000.0</v>
@@ -1584,34 +1602,34 @@
         <v>38.0</v>
       </c>
       <c r="B29" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D29" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E29" t="n">
         <v>20.0</v>
       </c>
       <c r="F29" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="G29" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H29" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="I29" t="s">
         <v>7</v>
       </c>
       <c r="J29" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="K29" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L29" t="n">
         <v>60000.0</v>
@@ -1628,34 +1646,34 @@
         <v>39.0</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D30" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E30" t="n">
         <v>20.0</v>
       </c>
       <c r="F30" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="G30" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="H30" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="I30" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J30" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="K30" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="L30" t="n">
         <v>100000.0</v>
@@ -1672,34 +1690,34 @@
         <v>40.0</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D31" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E31" t="n">
         <v>10.0</v>
       </c>
       <c r="F31" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="G31" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="H31" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="I31" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="J31" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="K31" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="L31" t="n">
         <v>100000.0</v>
@@ -1716,34 +1734,34 @@
         <v>41.0</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D32" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E32" t="n">
         <v>12.0</v>
       </c>
       <c r="F32" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G32" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="H32" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="I32" t="s">
         <v>7</v>
       </c>
       <c r="J32" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="K32" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="L32" t="n">
         <v>120000.0</v>
@@ -1760,34 +1778,34 @@
         <v>42.0</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D33" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E33" t="n">
         <v>12.0</v>
       </c>
       <c r="F33" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G33" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="H33" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="I33" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J33" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="K33" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="L33" t="n">
         <v>120000.0</v>
@@ -1804,34 +1822,34 @@
         <v>43.0</v>
       </c>
       <c r="B34" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C34" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D34" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E34" t="n">
         <v>9.0</v>
       </c>
       <c r="F34" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G34" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="H34" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="I34" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="J34" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="K34" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="L34" t="n">
         <v>150000.0</v>
@@ -1848,34 +1866,34 @@
         <v>44.0</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C35" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D35" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E35" t="n">
-        <v>31.0</v>
+        <v>3.0</v>
       </c>
       <c r="F35" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="G35" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="H35" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="I35" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J35" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="K35" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L35" t="n">
         <v>100000.0</v>
@@ -1892,40 +1910,40 @@
         <v>45.0</v>
       </c>
       <c r="B36" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C36" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D36" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E36" t="n">
-        <v>3.0</v>
+        <v>20.0</v>
       </c>
       <c r="F36" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G36" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="H36" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I36" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J36" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="K36" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="L36" t="n">
-        <v>60000.0</v>
+        <v>120000.0</v>
       </c>
       <c r="M36" t="n">
-        <v>60000.0</v>
+        <v>180000.0</v>
       </c>
       <c r="N36" t="b">
         <v>1</v>
@@ -1936,7 +1954,7 @@
         <v>46.0</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
       <c r="C37" t="s">
         <v>2</v>
@@ -1945,7 +1963,7 @@
         <v>3</v>
       </c>
       <c r="E37" t="n">
-        <v>21.0</v>
+        <v>3.0</v>
       </c>
       <c r="F37" t="s">
         <v>4</v>
@@ -1966,10 +1984,10 @@
         <v>9</v>
       </c>
       <c r="L37" t="n">
-        <v>70000.0</v>
+        <v>40000.0</v>
       </c>
       <c r="M37" t="n">
-        <v>70000.0</v>
+        <v>60000.0</v>
       </c>
       <c r="N37" t="b">
         <v>1</v>
@@ -1980,40 +1998,40 @@
         <v>47.0</v>
       </c>
       <c r="B38" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C38" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D38" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E38" t="n">
-        <v>9999.0</v>
+        <v>20.0</v>
       </c>
       <c r="F38" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="G38" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="H38" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I38" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="J38" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="K38" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="L38" t="n">
-        <v>70000.0</v>
+        <v>120000.0</v>
       </c>
       <c r="M38" t="n">
-        <v>70000.0</v>
+        <v>180000.0</v>
       </c>
       <c r="N38" t="b">
         <v>1</v>
@@ -2024,40 +2042,40 @@
         <v>48.0</v>
       </c>
       <c r="B39" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C39" t="s">
-        <v>98</v>
+        <v>11</v>
       </c>
       <c r="D39" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E39" t="n">
-        <v>1000.0</v>
+        <v>20.0</v>
       </c>
       <c r="F39" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G39" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="H39" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I39" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="J39" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="K39" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="L39" t="n">
-        <v>1000.0</v>
+        <v>120000.0</v>
       </c>
       <c r="M39" t="n">
-        <v>1000.0</v>
+        <v>180000.0</v>
       </c>
       <c r="N39" t="b">
         <v>1</v>
@@ -2068,40 +2086,40 @@
         <v>49.0</v>
       </c>
       <c r="B40" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C40" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D40" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E40" t="n">
-        <v>10.0</v>
+        <v>20.0</v>
       </c>
       <c r="F40" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="G40" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="H40" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I40" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J40" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="K40" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L40" t="n">
         <v>120000.0</v>
       </c>
       <c r="M40" t="n">
-        <v>280000.0</v>
+        <v>180000.0</v>
       </c>
       <c r="N40" t="b">
         <v>1</v>
@@ -2112,40 +2130,40 @@
         <v>50.0</v>
       </c>
       <c r="B41" t="s">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="C41" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D41" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E41" t="n">
-        <v>111101.0</v>
+        <v>20.0</v>
       </c>
       <c r="F41" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="G41" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="H41" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I41" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J41" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="K41" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L41" t="n">
         <v>120000.0</v>
       </c>
       <c r="M41" t="n">
-        <v>222222.0</v>
+        <v>180000.0</v>
       </c>
       <c r="N41" t="b">
         <v>1</v>
@@ -2156,40 +2174,40 @@
         <v>51.0</v>
       </c>
       <c r="B42" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="C42" t="s">
-        <v>102</v>
+        <v>11</v>
       </c>
       <c r="D42" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E42" t="n">
-        <v>1111112.0</v>
+        <v>20.0</v>
       </c>
       <c r="F42" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="G42" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="H42" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I42" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J42" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="K42" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L42" t="n">
         <v>120000.0</v>
       </c>
       <c r="M42" t="n">
-        <v>888888.0</v>
+        <v>180000.0</v>
       </c>
       <c r="N42" t="b">
         <v>1</v>
@@ -2200,40 +2218,40 @@
         <v>52.0</v>
       </c>
       <c r="B43" t="s">
-        <v>103</v>
+        <v>32</v>
       </c>
       <c r="C43" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D43" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E43" t="n">
-        <v>14.0</v>
+        <v>20.0</v>
       </c>
       <c r="F43" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G43" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H43" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I43" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="J43" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="K43" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L43" t="n">
-        <v>100000.0</v>
+        <v>120000.0</v>
       </c>
       <c r="M43" t="n">
-        <v>150000.0</v>
+        <v>180000.0</v>
       </c>
       <c r="N43" t="b">
         <v>1</v>
@@ -2244,40 +2262,40 @@
         <v>53.0</v>
       </c>
       <c r="B44" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C44" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="E44" t="n">
-        <v>14.0</v>
+        <v>101111.0</v>
       </c>
       <c r="F44" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="G44" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="H44" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="I44" t="s">
         <v>7</v>
       </c>
       <c r="J44" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="K44" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="L44" t="n">
-        <v>100000.0</v>
+        <v>40000.0</v>
       </c>
       <c r="M44" t="n">
-        <v>150000.0</v>
+        <v>60000.0</v>
       </c>
       <c r="N44" t="b">
         <v>1</v>
@@ -2288,40 +2306,40 @@
         <v>54.0</v>
       </c>
       <c r="B45" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="C45" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D45" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E45" t="n">
-        <v>14.0</v>
+        <v>10.0</v>
       </c>
       <c r="F45" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="G45" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H45" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I45" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="J45" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K45" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="L45" t="n">
-        <v>100000.0</v>
+        <v>90000.0</v>
       </c>
       <c r="M45" t="n">
-        <v>150000.0</v>
+        <v>135000.0</v>
       </c>
       <c r="N45" t="b">
         <v>1</v>
@@ -2332,40 +2350,40 @@
         <v>55.0</v>
       </c>
       <c r="B46" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="C46" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D46" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E46" t="n">
-        <v>14.0</v>
+        <v>20123.0</v>
       </c>
       <c r="F46" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G46" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H46" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I46" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="J46" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="K46" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L46" t="n">
-        <v>100000.0</v>
+        <v>120000.0</v>
       </c>
       <c r="M46" t="n">
-        <v>150000.0</v>
+        <v>180000.0</v>
       </c>
       <c r="N46" t="b">
         <v>1</v>
@@ -2376,40 +2394,40 @@
         <v>56.0</v>
       </c>
       <c r="B47" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C47" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D47" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E47" t="n">
-        <v>14.0</v>
+        <v>20123.0</v>
       </c>
       <c r="F47" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G47" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H47" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I47" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="J47" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="K47" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L47" t="n">
-        <v>100000.0</v>
+        <v>120000.0</v>
       </c>
       <c r="M47" t="n">
-        <v>150000.0</v>
+        <v>180000.0</v>
       </c>
       <c r="N47" t="b">
         <v>1</v>
@@ -2420,40 +2438,40 @@
         <v>57.0</v>
       </c>
       <c r="B48" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="C48" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D48" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E48" t="n">
-        <v>14.0</v>
+        <v>1.0</v>
       </c>
       <c r="F48" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G48" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H48" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I48" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="J48" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="K48" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L48" t="n">
-        <v>100000.0</v>
+        <v>120000.0</v>
       </c>
       <c r="M48" t="n">
-        <v>150000.0</v>
+        <v>180000.0</v>
       </c>
       <c r="N48" t="b">
         <v>1</v>
@@ -2464,42 +2482,790 @@
         <v>58.0</v>
       </c>
       <c r="B49" t="s">
+        <v>31</v>
+      </c>
+      <c r="C49" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F49" t="s">
+        <v>21</v>
+      </c>
+      <c r="G49" t="s">
+        <v>14</v>
+      </c>
+      <c r="H49" t="s">
+        <v>15</v>
+      </c>
+      <c r="I49" t="s">
+        <v>24</v>
+      </c>
+      <c r="J49" t="s">
+        <v>17</v>
+      </c>
+      <c r="K49" t="s">
+        <v>26</v>
+      </c>
+      <c r="L49" t="n">
+        <v>120000.0</v>
+      </c>
+      <c r="M49" t="n">
+        <v>180000.0</v>
+      </c>
+      <c r="N49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>59.0</v>
+      </c>
+      <c r="B50" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F50" t="s">
+        <v>13</v>
+      </c>
+      <c r="G50" t="s">
+        <v>14</v>
+      </c>
+      <c r="H50" t="s">
+        <v>15</v>
+      </c>
+      <c r="I50" t="s">
+        <v>16</v>
+      </c>
+      <c r="J50" t="s">
+        <v>17</v>
+      </c>
+      <c r="K50" t="s">
+        <v>9</v>
+      </c>
+      <c r="L50" t="n">
+        <v>120000.0</v>
+      </c>
+      <c r="M50" t="n">
+        <v>180000.0</v>
+      </c>
+      <c r="N50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>60.0</v>
+      </c>
+      <c r="B51" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>13</v>
+      </c>
+      <c r="G51" t="s">
+        <v>14</v>
+      </c>
+      <c r="H51" t="s">
+        <v>15</v>
+      </c>
+      <c r="I51" t="s">
+        <v>16</v>
+      </c>
+      <c r="J51" t="s">
+        <v>17</v>
+      </c>
+      <c r="K51" t="s">
+        <v>9</v>
+      </c>
+      <c r="L51" t="n">
+        <v>120000.0</v>
+      </c>
+      <c r="M51" t="n">
+        <v>180000.0</v>
+      </c>
+      <c r="N51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>61.0</v>
+      </c>
+      <c r="B52" t="s">
+        <v>98</v>
+      </c>
+      <c r="C52" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F52" t="s">
+        <v>13</v>
+      </c>
+      <c r="G52" t="s">
+        <v>14</v>
+      </c>
+      <c r="H52" t="s">
+        <v>15</v>
+      </c>
+      <c r="I52" t="s">
+        <v>16</v>
+      </c>
+      <c r="J52" t="s">
+        <v>17</v>
+      </c>
+      <c r="K52" t="s">
+        <v>9</v>
+      </c>
+      <c r="L52" t="n">
+        <v>120000.0</v>
+      </c>
+      <c r="M52" t="n">
+        <v>180000.0</v>
+      </c>
+      <c r="N52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>62.0</v>
+      </c>
+      <c r="B53" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" t="s">
+        <v>12</v>
+      </c>
+      <c r="E53" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F53" t="s">
+        <v>13</v>
+      </c>
+      <c r="G53" t="s">
+        <v>14</v>
+      </c>
+      <c r="H53" t="s">
+        <v>15</v>
+      </c>
+      <c r="I53" t="s">
+        <v>16</v>
+      </c>
+      <c r="J53" t="s">
+        <v>17</v>
+      </c>
+      <c r="K53" t="s">
+        <v>9</v>
+      </c>
+      <c r="L53" t="n">
+        <v>120000.0</v>
+      </c>
+      <c r="M53" t="n">
+        <v>180000.0</v>
+      </c>
+      <c r="N53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>63.0</v>
+      </c>
+      <c r="B54" t="s">
+        <v>100</v>
+      </c>
+      <c r="C54" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" t="s">
+        <v>12</v>
+      </c>
+      <c r="E54" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F54" t="s">
+        <v>13</v>
+      </c>
+      <c r="G54" t="s">
+        <v>14</v>
+      </c>
+      <c r="H54" t="s">
+        <v>15</v>
+      </c>
+      <c r="I54" t="s">
+        <v>16</v>
+      </c>
+      <c r="J54" t="s">
+        <v>17</v>
+      </c>
+      <c r="K54" t="s">
+        <v>9</v>
+      </c>
+      <c r="L54" t="n">
+        <v>120000.0</v>
+      </c>
+      <c r="M54" t="n">
+        <v>180000.0</v>
+      </c>
+      <c r="N54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>64.0</v>
+      </c>
+      <c r="B55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C55" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E55" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F55" t="s">
+        <v>13</v>
+      </c>
+      <c r="G55" t="s">
+        <v>14</v>
+      </c>
+      <c r="H55" t="s">
+        <v>15</v>
+      </c>
+      <c r="I55" t="s">
+        <v>16</v>
+      </c>
+      <c r="J55" t="s">
+        <v>17</v>
+      </c>
+      <c r="K55" t="s">
+        <v>9</v>
+      </c>
+      <c r="L55" t="n">
+        <v>120000.0</v>
+      </c>
+      <c r="M55" t="n">
+        <v>180000.0</v>
+      </c>
+      <c r="N55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>65.0</v>
+      </c>
+      <c r="B56" t="s">
+        <v>102</v>
+      </c>
+      <c r="C56" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" t="s">
+        <v>12</v>
+      </c>
+      <c r="E56" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F56" t="s">
+        <v>13</v>
+      </c>
+      <c r="G56" t="s">
+        <v>14</v>
+      </c>
+      <c r="H56" t="s">
+        <v>15</v>
+      </c>
+      <c r="I56" t="s">
+        <v>16</v>
+      </c>
+      <c r="J56" t="s">
+        <v>17</v>
+      </c>
+      <c r="K56" t="s">
+        <v>9</v>
+      </c>
+      <c r="L56" t="n">
+        <v>120000.0</v>
+      </c>
+      <c r="M56" t="n">
+        <v>180000.0</v>
+      </c>
+      <c r="N56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="B57" t="s">
+        <v>103</v>
+      </c>
+      <c r="C57" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57" t="s">
+        <v>12</v>
+      </c>
+      <c r="E57" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G57" t="s">
+        <v>14</v>
+      </c>
+      <c r="H57" t="s">
+        <v>15</v>
+      </c>
+      <c r="I57" t="s">
+        <v>16</v>
+      </c>
+      <c r="J57" t="s">
+        <v>17</v>
+      </c>
+      <c r="K57" t="s">
+        <v>9</v>
+      </c>
+      <c r="L57" t="n">
+        <v>120000.0</v>
+      </c>
+      <c r="M57" t="n">
+        <v>180000.0</v>
+      </c>
+      <c r="N57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>67.0</v>
+      </c>
+      <c r="B58" t="s">
+        <v>104</v>
+      </c>
+      <c r="C58" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" t="s">
+        <v>12</v>
+      </c>
+      <c r="E58" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F58" t="s">
+        <v>13</v>
+      </c>
+      <c r="G58" t="s">
+        <v>14</v>
+      </c>
+      <c r="H58" t="s">
+        <v>15</v>
+      </c>
+      <c r="I58" t="s">
+        <v>16</v>
+      </c>
+      <c r="J58" t="s">
+        <v>17</v>
+      </c>
+      <c r="K58" t="s">
+        <v>9</v>
+      </c>
+      <c r="L58" t="n">
+        <v>120000.0</v>
+      </c>
+      <c r="M58" t="n">
+        <v>180000.0</v>
+      </c>
+      <c r="N58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>68.0</v>
+      </c>
+      <c r="B59" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" t="s">
+        <v>12</v>
+      </c>
+      <c r="E59" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F59" t="s">
+        <v>13</v>
+      </c>
+      <c r="G59" t="s">
+        <v>14</v>
+      </c>
+      <c r="H59" t="s">
+        <v>15</v>
+      </c>
+      <c r="I59" t="s">
+        <v>16</v>
+      </c>
+      <c r="J59" t="s">
+        <v>17</v>
+      </c>
+      <c r="K59" t="s">
+        <v>9</v>
+      </c>
+      <c r="L59" t="n">
+        <v>120000.0</v>
+      </c>
+      <c r="M59" t="n">
+        <v>180000.0</v>
+      </c>
+      <c r="N59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>69.0</v>
+      </c>
+      <c r="B60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60" t="s">
+        <v>19</v>
+      </c>
+      <c r="D60" t="s">
+        <v>20</v>
+      </c>
+      <c r="E60" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F60" t="s">
+        <v>21</v>
+      </c>
+      <c r="G60" t="s">
+        <v>22</v>
+      </c>
+      <c r="H60" t="s">
+        <v>23</v>
+      </c>
+      <c r="I60" t="s">
+        <v>24</v>
+      </c>
+      <c r="J60" t="s">
         <v>25</v>
       </c>
-      <c r="C49" t="s">
-        <v>18</v>
-      </c>
-      <c r="D49" t="s">
-        <v>19</v>
-      </c>
-      <c r="E49" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="F49" t="s">
-        <v>20</v>
-      </c>
-      <c r="G49" t="s">
+      <c r="K60" t="s">
+        <v>26</v>
+      </c>
+      <c r="L60" t="n">
+        <v>100000.0</v>
+      </c>
+      <c r="M60" t="n">
+        <v>150000.0</v>
+      </c>
+      <c r="N60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="B61" t="s">
+        <v>105</v>
+      </c>
+      <c r="C61" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" t="s">
+        <v>106</v>
+      </c>
+      <c r="E61" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="F61" t="s">
+        <v>51</v>
+      </c>
+      <c r="G61" t="s">
+        <v>107</v>
+      </c>
+      <c r="H61" t="s">
+        <v>108</v>
+      </c>
+      <c r="I61" t="s">
+        <v>7</v>
+      </c>
+      <c r="J61" t="s">
+        <v>8</v>
+      </c>
+      <c r="K61" t="s">
+        <v>39</v>
+      </c>
+      <c r="L61" t="n">
+        <v>120000.0</v>
+      </c>
+      <c r="M61" t="n">
+        <v>180000.0</v>
+      </c>
+      <c r="N61" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>71.0</v>
+      </c>
+      <c r="B62" t="s">
+        <v>109</v>
+      </c>
+      <c r="C62" t="s">
+        <v>11</v>
+      </c>
+      <c r="D62" t="s">
+        <v>106</v>
+      </c>
+      <c r="E62" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="F62" t="s">
+        <v>51</v>
+      </c>
+      <c r="G62" t="s">
+        <v>107</v>
+      </c>
+      <c r="H62" t="s">
+        <v>108</v>
+      </c>
+      <c r="I62" t="s">
+        <v>7</v>
+      </c>
+      <c r="J62" t="s">
+        <v>8</v>
+      </c>
+      <c r="K62" t="s">
+        <v>39</v>
+      </c>
+      <c r="L62" t="n">
+        <v>120000.0</v>
+      </c>
+      <c r="M62" t="n">
+        <v>180000.0</v>
+      </c>
+      <c r="N62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="B63" t="s">
+        <v>110</v>
+      </c>
+      <c r="C63" t="s">
+        <v>11</v>
+      </c>
+      <c r="D63" t="s">
+        <v>12</v>
+      </c>
+      <c r="E63" t="n">
+        <v>111.0</v>
+      </c>
+      <c r="F63" t="s">
         <v>21</v>
       </c>
-      <c r="H49" t="s">
-        <v>22</v>
-      </c>
-      <c r="I49" t="s">
+      <c r="G63" t="s">
+        <v>14</v>
+      </c>
+      <c r="H63" t="s">
+        <v>15</v>
+      </c>
+      <c r="I63" t="s">
+        <v>24</v>
+      </c>
+      <c r="J63" t="s">
+        <v>17</v>
+      </c>
+      <c r="K63" t="s">
+        <v>26</v>
+      </c>
+      <c r="L63" t="n">
+        <v>120000.0</v>
+      </c>
+      <c r="M63" t="n">
+        <v>180000.0</v>
+      </c>
+      <c r="N63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>73.0</v>
+      </c>
+      <c r="B64" t="s">
+        <v>111</v>
+      </c>
+      <c r="C64" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" t="s">
+        <v>12</v>
+      </c>
+      <c r="E64" t="n">
+        <v>1111111.0</v>
+      </c>
+      <c r="F64" t="s">
+        <v>21</v>
+      </c>
+      <c r="G64" t="s">
+        <v>14</v>
+      </c>
+      <c r="H64" t="s">
+        <v>15</v>
+      </c>
+      <c r="I64" t="s">
+        <v>24</v>
+      </c>
+      <c r="J64" t="s">
+        <v>17</v>
+      </c>
+      <c r="K64" t="s">
+        <v>26</v>
+      </c>
+      <c r="L64" t="n">
+        <v>120000.0</v>
+      </c>
+      <c r="M64" t="n">
+        <v>180000.0</v>
+      </c>
+      <c r="N64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>74.0</v>
+      </c>
+      <c r="B65" t="s">
+        <v>112</v>
+      </c>
+      <c r="C65" t="s">
+        <v>11</v>
+      </c>
+      <c r="D65" t="s">
+        <v>12</v>
+      </c>
+      <c r="E65" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="F65" t="s">
+        <v>13</v>
+      </c>
+      <c r="G65" t="s">
+        <v>14</v>
+      </c>
+      <c r="H65" t="s">
+        <v>15</v>
+      </c>
+      <c r="I65" t="s">
+        <v>24</v>
+      </c>
+      <c r="J65" t="s">
+        <v>17</v>
+      </c>
+      <c r="K65" t="s">
+        <v>26</v>
+      </c>
+      <c r="L65" t="n">
+        <v>120000.0</v>
+      </c>
+      <c r="M65" t="n">
+        <v>180000.0</v>
+      </c>
+      <c r="N65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>75.0</v>
+      </c>
+      <c r="B66" t="s">
+        <v>113</v>
+      </c>
+      <c r="C66" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66" t="s">
+        <v>12</v>
+      </c>
+      <c r="E66" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="F66" t="s">
+        <v>59</v>
+      </c>
+      <c r="G66" t="s">
+        <v>14</v>
+      </c>
+      <c r="H66" t="s">
+        <v>15</v>
+      </c>
+      <c r="I66" t="s">
         <v>7</v>
       </c>
-      <c r="J49" t="s">
-        <v>23</v>
-      </c>
-      <c r="K49" t="s">
-        <v>24</v>
-      </c>
-      <c r="L49" t="n">
-        <v>100000.0</v>
-      </c>
-      <c r="M49" t="n">
-        <v>150000.0</v>
-      </c>
-      <c r="N49" t="b">
+      <c r="J66" t="s">
+        <v>17</v>
+      </c>
+      <c r="K66" t="s">
+        <v>26</v>
+      </c>
+      <c r="L66" t="n">
+        <v>120000.0</v>
+      </c>
+      <c r="M66" t="n">
+        <v>180000.0</v>
+      </c>
+      <c r="N66" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>